<commit_message>
[FIX]pabi_budget_xls: changed label in excel template ref:/issues/1302#note-5
</commit_message>
<xml_diff>
--- a/pabi_budget_xls/template/Template_Section_Plan_23_nov.xlsx
+++ b/pabi_budget_xls/template/Template_Section_Plan_23_nov.xlsx
@@ -5,21 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="724" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="724" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Section" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="ActivityGroup_MasterData" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="CostControl_MasterData" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Non_CostControl" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="CostControl_1" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="master_section" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="master_activity_group" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="master_job_order" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Non_jobOrder" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="JobOrder" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="136">
   <si>
     <t>Org</t>
   </si>
@@ -350,7 +350,7 @@
   </si>
   <si>
     <t>Auto-Calc
-G*H*I</t>
+D*E*F</t>
   </si>
   <si>
     <t>Previous year commitment</t>
@@ -442,7 +442,11 @@
     <t>Check</t>
   </si>
   <si>
-    <t>Cost Control</t>
+    <t>Job Order</t>
+  </si>
+  <si>
+    <t>Auto-Calc
+G*H*I</t>
   </si>
   <si>
     <t>Auto-Calc
@@ -1183,7 +1187,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1511,7 +1515,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1567,8 +1571,8 @@
   </sheetPr>
   <dimension ref="1:10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10989,8 +10993,8 @@
   </sheetPr>
   <dimension ref="1:185"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D176" activeCellId="0" sqref="D176"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A178" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C195" activeCellId="0" sqref="C195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -11131,7 +11135,7 @@
         <v>101</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="H10" s="19" t="s">
         <v>103</v>
@@ -11149,10 +11153,10 @@
       <c r="S10" s="17"/>
       <c r="T10" s="17"/>
       <c r="U10" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="V10" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11753,7 +11757,7 @@
         <v>101</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="H28" s="19" t="s">
         <v>103</v>
@@ -11771,10 +11775,10 @@
       <c r="S28" s="17"/>
       <c r="T28" s="17"/>
       <c r="U28" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="V28" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12355,7 +12359,7 @@
         <v>101</v>
       </c>
       <c r="G46" s="19" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="H46" s="19" t="s">
         <v>103</v>
@@ -12373,10 +12377,10 @@
       <c r="S46" s="17"/>
       <c r="T46" s="17"/>
       <c r="U46" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="V46" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12957,7 +12961,7 @@
         <v>101</v>
       </c>
       <c r="G64" s="19" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="H64" s="19" t="s">
         <v>103</v>
@@ -12975,10 +12979,10 @@
       <c r="S64" s="17"/>
       <c r="T64" s="17"/>
       <c r="U64" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="V64" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13559,7 +13563,7 @@
         <v>101</v>
       </c>
       <c r="G82" s="19" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="H82" s="19" t="s">
         <v>103</v>
@@ -13577,10 +13581,10 @@
       <c r="S82" s="17"/>
       <c r="T82" s="17"/>
       <c r="U82" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="V82" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14161,7 +14165,7 @@
         <v>101</v>
       </c>
       <c r="G100" s="19" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="H100" s="19" t="s">
         <v>103</v>
@@ -14179,10 +14183,10 @@
       <c r="S100" s="17"/>
       <c r="T100" s="17"/>
       <c r="U100" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="V100" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14763,7 +14767,7 @@
         <v>101</v>
       </c>
       <c r="G118" s="19" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="H118" s="19" t="s">
         <v>103</v>
@@ -14781,10 +14785,10 @@
       <c r="S118" s="17"/>
       <c r="T118" s="17"/>
       <c r="U118" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="V118" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15365,7 +15369,7 @@
         <v>101</v>
       </c>
       <c r="G136" s="19" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="H136" s="19" t="s">
         <v>103</v>
@@ -15383,10 +15387,10 @@
       <c r="S136" s="17"/>
       <c r="T136" s="17"/>
       <c r="U136" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="V136" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15967,7 +15971,7 @@
         <v>101</v>
       </c>
       <c r="G154" s="19" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="H154" s="19" t="s">
         <v>103</v>
@@ -15985,10 +15989,10 @@
       <c r="S154" s="17"/>
       <c r="T154" s="17"/>
       <c r="U154" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="V154" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16569,7 +16573,7 @@
         <v>101</v>
       </c>
       <c r="G172" s="19" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="H172" s="19" t="s">
         <v>103</v>
@@ -16587,10 +16591,10 @@
       <c r="S172" s="17"/>
       <c r="T172" s="17"/>
       <c r="U172" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="V172" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17145,7 +17149,7 @@
   </mergeCells>
   <dataValidations count="2">
     <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B8 B26 B44 B62 B80 B98 B116 B134 B152 B170" type="list">
-      <formula1>CostControl_MasterData!$C$2:$C$208</formula1>
+      <formula1>master_job_order!$C$2:$C$208</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D13:F22 I13:T22 D31:F40 I31:T40 D49:F58 I49:T58 D67:F76 I67:T76 D85:F94 I85:T94 D103:F112 I103:T112 D121:F130 I121:T130 D139:F148 I139:T148 D157:F166 I157:T166 D175:F184 I175:T184" type="decimal">

</xml_diff>

<commit_message>
[IMP]pabi_budget_xls: added external/internal expense/revenue for import/export excel ref:issues/1307
</commit_message>
<xml_diff>
--- a/pabi_budget_xls/template/Template_Section_Plan_23_nov.xlsx
+++ b/pabi_budget_xls/template/Template_Section_Plan_23_nov.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="724" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="724" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Non_JobOrder_Expense" sheetId="1" state="visible" r:id="rId2"/>
@@ -954,7 +954,7 @@
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF00CC00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -1021,7 +1021,7 @@
   <dimension ref="1:10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="1" sqref="J13:U13 A21"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10446,13 +10446,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFF00"/>
+    <tabColor rgb="FF00CC00"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="J13:U13 A8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -19882,8 +19882,8 @@
   </sheetPr>
   <dimension ref="1:285"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13:U13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -29642,7 +29642,7 @@
   <dimension ref="A2:I207"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="J13:U13 C14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -30147,7 +30147,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="1" sqref="J13:U13 A32"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -30176,7 +30176,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="1" sqref="J13:U13 A24"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>